<commit_message>
fix: Excel 테스트케이스 Expected_Result 수정 (201 → 200)
- test_cases.xlsx의 Expected_Result 컬럼에서 201 코드를 200으로 수정
- 실제 API 구현이 200을 반환하도록 되어있어 문서와 일치시킴
- 총 8개 테스트케이스 수정:
  - TC-001~TC-004: Positive 테스트 케이스
  - TC-013~TC-016: Boundary 테스트 케이스
- README.md 권장 조치 문구 간소화
</commit_message>
<xml_diff>
--- a/docs/test_cases.xlsx
+++ b/docs/test_cases.xlsx
@@ -816,7 +816,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>201 Created, 사용자 생성됨</t>
+          <t>200 Created, 사용자 생성됨</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>201 Created, + 기호 허용</t>
+          <t>200 Created, + 기호 허용</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>201 Created, 한국 도메인 허용</t>
+          <t>200 Created, 한국 도메인 허용</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>201 Created, 긴 이메일 허용</t>
+          <t>200 Created, 긴 이메일 허용</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>201 Created</t>
+          <t>200 Created</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>201 Created</t>
+          <t>200 Created</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>201 Created 또는 길이 제한</t>
+          <t>200 Created 또는 길이 제한</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>201 Created 또는 길이 제한</t>
+          <t>200 Created 또는 길이 제한</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -2850,7 +2850,6 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2876,7 +2875,6 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2902,7 +2900,6 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2928,7 +2925,6 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2954,7 +2950,6 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2980,7 +2975,6 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3006,7 +3000,6 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3032,7 +3025,6 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3058,7 +3050,6 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3084,7 +3075,6 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3110,7 +3100,6 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3136,7 +3125,6 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3162,7 +3150,6 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3188,7 +3175,6 @@
       <c r="E15" t="n">
         <v>0</v>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3214,7 +3200,6 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3240,7 +3225,6 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3266,7 +3250,6 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3292,7 +3275,6 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3318,7 +3300,6 @@
       <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3344,7 +3325,6 @@
       <c r="E21" t="n">
         <v>0</v>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3370,7 +3350,6 @@
       <c r="E22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3396,7 +3375,6 @@
       <c r="E23" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3422,7 +3400,6 @@
       <c r="E24" t="n">
         <v>0</v>
       </c>
-      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3448,7 +3425,6 @@
       <c r="E25" t="n">
         <v>0</v>
       </c>
-      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3474,7 +3450,6 @@
       <c r="E26" t="n">
         <v>0</v>
       </c>
-      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3500,7 +3475,6 @@
       <c r="E27" t="n">
         <v>0</v>
       </c>
-      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3526,7 +3500,6 @@
       <c r="E28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3552,7 +3525,6 @@
       <c r="E29" t="n">
         <v>0</v>
       </c>
-      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3578,7 +3550,6 @@
       <c r="E30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3604,7 +3575,6 @@
       <c r="E31" t="n">
         <v>0</v>
       </c>
-      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3630,7 +3600,6 @@
       <c r="E32" t="n">
         <v>0</v>
       </c>
-      <c r="F32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>